<commit_message>
Added features and README file
</commit_message>
<xml_diff>
--- a/financials.xlsx
+++ b/financials.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hhmp2\Desktop\Placement Resources\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hhmp2\Desktop\Placement Resources\Project\financial-statement-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9264" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9264" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Income Statement" sheetId="1" r:id="rId1"/>
-    <sheet name="Balance sheet" sheetId="2" r:id="rId2"/>
+    <sheet name="Balance Sheet" sheetId="2" r:id="rId2"/>
     <sheet name="Cash Flow Statement" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -64,9 +64,6 @@
     <t>Total Liabilities</t>
   </si>
   <si>
-    <t>Shareholders' Equity</t>
-  </si>
-  <si>
     <t>Cash flow from Operating Activities</t>
   </si>
   <si>
@@ -74,6 +71,9 @@
   </si>
   <si>
     <t>Cash flow from Financing Activities</t>
+  </si>
+  <si>
+    <t>Shareholders Equity</t>
   </si>
 </sst>
 </file>
@@ -521,8 +521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -588,7 +588,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B6" s="3">
         <v>65398</v>
@@ -606,7 +606,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -629,7 +629,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" s="3">
         <v>18009</v>
@@ -640,7 +640,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="3">
         <v>-3573</v>
@@ -651,7 +651,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="3">
         <v>-15881</v>

</xml_diff>